<commit_message>
Updatd the command strings file to reflect changes to the drivertain.
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD1E4F-4009-4A15-B3E1-B23327364584}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="8424"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -173,22 +174,19 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Two Digit Positive Number 00 to 99</t>
-  </si>
-  <si>
-    <t>00 to 99 + 00 to 99</t>
-  </si>
-  <si>
-    <t>"D1575"</t>
-  </si>
-  <si>
-    <t>&lt; 50 is backwards, and &gt; 50 is forwards. First two digits are for the left side, last two are for the right side.</t>
+    <t>left,right</t>
+  </si>
+  <si>
+    <t>negative is backwards, and positive is forwards. Range is ±100</t>
+  </si>
+  <si>
+    <t>"D-40,40"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,28 +543,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="6" width="31.88671875" customWidth="1"/>
-    <col min="7" max="7" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="33.6640625" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" customWidth="1"/>
-    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -595,7 +593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -605,9 +603,6 @@
       <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
       <c r="J3" t="s">
         <v>33</v>
       </c>
@@ -621,7 +616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="58.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -635,10 +630,10 @@
         <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>51</v>
@@ -656,7 +651,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
@@ -677,7 +672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
@@ -698,7 +693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
@@ -713,7 +708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
@@ -721,7 +716,7 @@
       <c r="E8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -741,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="58.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
@@ -759,7 +754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="6" t="s">
         <v>17</v>
@@ -777,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="6" t="s">
         <v>18</v>
@@ -795,7 +790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="6" t="s">
         <v>45</v>
@@ -809,7 +804,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="6" t="s">
         <v>45</v>
@@ -823,7 +818,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -831,7 +826,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -849,7 +844,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
         <v>12</v>
@@ -867,7 +862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
@@ -885,7 +880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
@@ -899,19 +894,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated the command strings to include GPS endpoint
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD1E4F-4009-4A15-B3E1-B23327364584}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676F0746-7594-400C-A6F6-01E83563C5A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -181,6 +181,27 @@
   </si>
   <si>
     <t>"D-40,40"</t>
+  </si>
+  <si>
+    <t>Rover Systems</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Receive GPS Stream</t>
+  </si>
+  <si>
+    <t>Response Format</t>
+  </si>
+  <si>
+    <t>lat,long,alt,speed,heading,satellites</t>
+  </si>
+  <si>
+    <t>Example Response</t>
+  </si>
+  <si>
+    <t>Simply open the conenction to receive data</t>
   </si>
 </sst>
 </file>
@@ -544,371 +565,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M23"/>
+  <dimension ref="A2:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="6" width="31.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="33.7109375" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="10" max="12" width="29.42578125" customWidth="1"/>
+    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="16" max="16" width="33.7109375" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
+      <c r="P3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
         <v>37</v>
       </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>9001</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C9">
+        <v>9002</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="J6" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F14" s="1">
         <v>50</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6" t="s">
+    <row r="15" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F15" s="1">
         <v>50</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6" t="s">
+    <row r="16" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <v>50</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1">
+        <v>50</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>50</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F22" s="1">
         <v>50</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" t="s">
+      <c r="G23" s="2"/>
+      <c r="H23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E19">
+      <c r="F24">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the command strings to match development progress
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676F0746-7594-400C-A6F6-01E83563C5A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D348EEA-7AF6-4055-B373-B7DD852CFF41}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Command/Arm DOF</t>
   </si>
   <si>
-    <t>Drive Train</t>
-  </si>
-  <si>
     <t>Arm</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>"D-40,40"</t>
   </si>
   <si>
-    <t>Rover Systems</t>
-  </si>
-  <si>
     <t>Port</t>
   </si>
   <si>
@@ -202,6 +196,21 @@
   </si>
   <si>
     <t>Simply open the conenction to receive data</t>
+  </si>
+  <si>
+    <t>Receive Temperature Stream</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>0.000000000,0.0000000000,0.00,0.00,0.0,0</t>
+  </si>
+  <si>
+    <t>Rover Systems (8000-9000)</t>
+  </si>
+  <si>
+    <t>Drive Train (9000-10000)</t>
   </si>
 </sst>
 </file>
@@ -568,13 +577,13 @@
   <dimension ref="A2:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
@@ -582,7 +591,8 @@
     <col min="7" max="7" width="40.42578125" customWidth="1"/>
     <col min="8" max="8" width="29.42578125" customWidth="1"/>
     <col min="9" max="9" width="38.28515625" customWidth="1"/>
-    <col min="10" max="12" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="29.42578125" customWidth="1"/>
     <col min="15" max="15" width="24" customWidth="1"/>
     <col min="16" max="16" width="33.7109375" customWidth="1"/>
     <col min="17" max="17" width="26.85546875" customWidth="1"/>
@@ -597,41 +607,41 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="O2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
@@ -640,96 +650,121 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>8001</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
         <v>54</v>
       </c>
-      <c r="C5">
-        <v>9001</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>8002</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="I5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="J6">
+        <v>48.234000000000002</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="O6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
       <c r="R6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="O7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -738,28 +773,28 @@
     </row>
     <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>9002</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -819,88 +854,88 @@
     </row>
     <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1">
         <v>50</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1">
         <v>50</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1">
         <v>50</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="1">
         <v>50</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
@@ -908,13 +943,13 @@
     <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
@@ -929,67 +964,67 @@
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1">
         <v>50</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24">
         <v>50</v>

</xml_diff>

<commit_message>
Updated the command strings list
The arm is not currently consistent with the code, but that's because
the code is unfinished.
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D348EEA-7AF6-4055-B373-B7DD852CFF41}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B7836-2220-48B9-86DC-208575B42547}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -78,24 +78,9 @@
     <t>Elbow</t>
   </si>
   <si>
-    <t>Claw Linear Actuator</t>
-  </si>
-  <si>
     <t>Example Full String</t>
   </si>
   <si>
-    <t>50 is neutral, &lt;50 CCW, &gt;50 CW</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;50 is decreasing angle and &gt;50 Increasing angle  Angle is defined between arm and the top of the rover</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;50 is decreasing angle and &gt;50 Increasing. The angle is defined as between the two arm beams (&lt;=180)</t>
-  </si>
-  <si>
-    <t>&lt;50 is closing claw and &gt;50 opening</t>
-  </si>
-  <si>
     <t>Science</t>
   </si>
   <si>
@@ -159,15 +144,6 @@
     <t>Gateway</t>
   </si>
   <si>
-    <t>Placeholder Name</t>
-  </si>
-  <si>
-    <t>"E"</t>
-  </si>
-  <si>
-    <t>"F"</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -207,10 +183,73 @@
     <t>0.000000000,0.0000000000,0.00,0.00,0.0,0</t>
   </si>
   <si>
-    <t>Rover Systems (8000-9000)</t>
-  </si>
-  <si>
-    <t>Drive Train (9000-10000)</t>
+    <t>Rover Systems (8000-8999)</t>
+  </si>
+  <si>
+    <t>Drive Train (9000-9999)</t>
+  </si>
+  <si>
+    <t>Arm (10000-10999)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AR30</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>0 is stop, &lt;0 down, &gt;0 up</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>AL30</t>
+  </si>
+  <si>
+    <t>0 is stop, &lt;0 CCW, &gt;0 CW</t>
+  </si>
+  <si>
+    <t>AE30</t>
+  </si>
+  <si>
+    <t>Claw Pitch</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Claw Rotation</t>
+  </si>
+  <si>
+    <t>CP30</t>
+  </si>
+  <si>
+    <t>CR30</t>
+  </si>
+  <si>
+    <t>Claw Actuator</t>
+  </si>
+  <si>
+    <t>0 is stop, &lt;0 retract, &gt;0 extend</t>
+  </si>
+  <si>
+    <t>CC30</t>
   </si>
 </sst>
 </file>
@@ -574,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R28"/>
+  <dimension ref="A2:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,30 +649,30 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -641,7 +680,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
@@ -650,96 +689,96 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="Q3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>8001</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="Q5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>8002</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J6">
         <v>48.234000000000002</v>
@@ -748,23 +787,23 @@
         <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="Q6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -773,28 +812,28 @@
     </row>
     <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>9002</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -854,105 +893,149 @@
     </row>
     <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C14">
+        <v>10001</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="C15">
+        <v>10001</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1">
-        <v>50</v>
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="60.75" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C16">
+        <v>10001</v>
+      </c>
       <c r="D16" s="5" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="1">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>67</v>
+      </c>
+      <c r="C17">
+        <v>10001</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>69</v>
+      </c>
+      <c r="C18">
+        <v>10001</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <v>10001</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
@@ -963,76 +1046,80 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="1">
-        <v>50</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>50</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
@@ -1045,6 +1132,10 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update autonomous message formats
Updated autonomous command strings. Added message types for controlling
the autonomous system.
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Talonj123\MAVRIC\MAVRIC-Electrical\Control Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Documents\College\Iowa State\MAVRIC\MAVRIC-Systems\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B7836-2220-48B9-86DC-208575B42547}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC2AE60-41C9-4284-A843-B2541B569131}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="21720" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="21720" windowHeight="8436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -250,6 +250,45 @@
   </si>
   <si>
     <t>CC30</t>
+  </si>
+  <si>
+    <t>Autonomous</t>
+  </si>
+  <si>
+    <t>Next waypoint</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>lat,long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +lat is N, -lat is S; +long is E, -long is W               Values to 4 decimal places</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Enables autonomous, disables normal drive</t>
+  </si>
+  <si>
+    <t>Disables autonomous, enables normal drive</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>NW42.0308,-93.6319</t>
   </si>
 </sst>
 </file>
@@ -613,32 +652,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R29"/>
+  <dimension ref="A2:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
-    <col min="10" max="10" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="31.88671875" customWidth="1"/>
+    <col min="7" max="7" width="40.44140625" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
+    <col min="9" max="9" width="38.33203125" customWidth="1"/>
+    <col min="10" max="10" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="29.44140625" customWidth="1"/>
     <col min="15" max="15" width="24" customWidth="1"/>
-    <col min="16" max="16" width="33.7109375" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="33.6640625" customWidth="1"/>
+    <col min="17" max="17" width="26.88671875" customWidth="1"/>
+    <col min="18" max="18" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="36" x14ac:dyDescent="0.35">
       <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
@@ -675,7 +714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -701,7 +740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -720,7 +759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -758,7 +797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>49</v>
       </c>
@@ -796,7 +835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="O7" t="s">
@@ -806,11 +845,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -840,7 +879,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
       <c r="D10" s="5"/>
@@ -853,7 +892,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="D11" s="5"/>
@@ -866,7 +905,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="D12" s="5"/>
@@ -879,7 +918,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="D13" s="5"/>
@@ -891,7 +930,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
@@ -917,7 +956,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -941,7 +980,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
@@ -965,7 +1004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
         <v>67</v>
@@ -989,7 +1028,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
         <v>69</v>
@@ -1013,7 +1052,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
         <v>72</v>
@@ -1037,7 +1076,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="D20" s="5"/>
@@ -1045,7 +1084,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="D21" s="5"/>
@@ -1053,7 +1092,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1071,7 +1110,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
         <v>11</v>
@@ -1089,7 +1128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1121,21 +1160,84 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added radius turning, added waypoint clearing
Added functions to allow radius turning instead of point turning. Added
a command to erase all waypoints (useful for testing). Removed some
debug prints.
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Documents\College\Iowa State\MAVRIC\MAVRIC-Systems\Control Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC2AE60-41C9-4284-A843-B2541B569131}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC5A49-2D7B-49CC-8806-B259E69379C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="0" windowWidth="21720" windowHeight="8436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Example Response</t>
   </si>
   <si>
-    <t>Simply open the conenction to receive data</t>
-  </si>
-  <si>
     <t>Receive Temperature Stream</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>lat,long</t>
   </si>
   <si>
-    <t xml:space="preserve"> +lat is N, -lat is S; +long is E, -long is W               Values to 4 decimal places</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
@@ -288,7 +282,25 @@
     <t>W</t>
   </si>
   <si>
-    <t>NW42.0308,-93.6319</t>
+    <t>Forget waypoints</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>Erases (forgets) all waypoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +lat is N, -lat is S; +long is E, -long is W               Values to 6 decimal places</t>
+  </si>
+  <si>
+    <t>NW42.034534,-93.620369</t>
+  </si>
+  <si>
+    <t>Simply open the connection to receive data</t>
   </si>
 </sst>
 </file>
@@ -652,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R32"/>
+  <dimension ref="A2:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,7 +754,7 @@
     </row>
     <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -776,13 +788,13 @@
         <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
@@ -799,7 +811,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>8002</v>
@@ -814,10 +826,10 @@
         <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6">
         <v>48.234000000000002</v>
@@ -851,7 +863,7 @@
     </row>
     <row r="9" spans="1:18" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -860,7 +872,7 @@
         <v>9002</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>39</v>
@@ -932,7 +944,7 @@
     </row>
     <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
@@ -941,19 +953,19 @@
         <v>10001</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
         <v>58</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -965,19 +977,19 @@
         <v>10001</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
         <v>63</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -989,91 +1001,91 @@
         <v>10001</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>10001</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18">
         <v>10001</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>10001</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" t="s">
         <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -1178,65 +1190,85 @@
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G31" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H31" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" t="s">
         <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
         <v>83</v>
+      </c>
+      <c r="H33" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated command strings for steer
</commit_message>
<xml_diff>
--- a/Control Systems/Command Strings List.xlsx
+++ b/Control Systems/Command Strings List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Documents\College\Iowa State\MAVRIC\MAVRIC-Systems\Control Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\Junior 2nd semester\AER 494\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC5A49-2D7B-49CC-8806-B259E69379C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC4FA8E-0502-454F-9613-33C8973AD992}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="21720" windowHeight="8436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
   <si>
     <t>SubSystem Code</t>
   </si>
@@ -96,9 +96,6 @@
     <t>2nd Actuator</t>
   </si>
   <si>
-    <t>Both Side</t>
-  </si>
-  <si>
     <t>"SC75"</t>
   </si>
   <si>
@@ -301,6 +298,33 @@
   </si>
   <si>
     <t>Simply open the connection to receive data</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Steer</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Range is ±90</t>
+  </si>
+  <si>
+    <t>steer left, steer right</t>
+  </si>
+  <si>
+    <t>"S45,-45"</t>
+  </si>
+  <si>
+    <t>Steer Feedback</t>
+  </si>
+  <si>
+    <t>left front, left back, right front, right back</t>
+  </si>
+  <si>
+    <t>0.0,0.0,0.0,0.0</t>
   </si>
 </sst>
 </file>
@@ -666,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,24 +730,24 @@
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -731,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
@@ -740,96 +764,96 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>8001</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>8002</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <v>48.234000000000002</v>
@@ -838,23 +862,23 @@
         <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="O7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -863,28 +887,28 @@
     </row>
     <row r="9" spans="1:18" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>9002</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -893,12 +917,27 @@
     </row>
     <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>9002</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -906,14 +945,31 @@
     </row>
     <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11">
+        <v>9004</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
@@ -944,7 +1000,7 @@
     </row>
     <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>14</v>
@@ -953,19 +1009,19 @@
         <v>10001</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
         <v>57</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -977,19 +1033,19 @@
         <v>10001</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
         <v>62</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -1001,91 +1057,91 @@
         <v>10001</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>10001</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>10001</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19">
         <v>10001</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
         <v>72</v>
-      </c>
-      <c r="H19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -1155,7 +1211,7 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1190,85 +1246,97 @@
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C30">
+        <v>9004</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="C31">
+        <v>9003</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" t="s">
         <v>89</v>
-      </c>
-      <c r="H31" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32">
+        <v>9003</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" t="s">
         <v>86</v>
-      </c>
-      <c r="F32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33">
+        <v>9003</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>